<commit_message>
updated puerto rico stochastics
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/scenarios.xlsx
+++ b/projects/puerto_rico_stoch/data/scenarios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCAE105-6654-4C92-AF06-F36B7AFC56C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC094175-12AF-451D-B7AD-80551F112D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SolverSettings" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="75">
   <si>
     <t>Scenario</t>
   </si>
@@ -236,6 +236,18 @@
   </si>
   <si>
     <t>ZB</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>YC</t>
+  </si>
+  <si>
+    <t>ZC</t>
   </si>
 </sst>
 </file>
@@ -251,12 +263,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,10 +289,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,7 +586,7 @@
     <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,28 +606,40 @@
         <v>63</v>
       </c>
       <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
         <v>69</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -648,8 +679,20 @@
       <c r="M2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -689,8 +732,20 @@
       <c r="M3" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -730,8 +785,20 @@
       <c r="M4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -771,8 +838,20 @@
       <c r="M5" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -812,8 +891,20 @@
       <c r="M6" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -853,8 +944,20 @@
       <c r="M7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7">
+        <v>100</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -894,8 +997,20 @@
       <c r="M8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>1000</v>
+      </c>
+      <c r="O8">
+        <v>1000</v>
+      </c>
+      <c r="P8">
+        <v>1000</v>
+      </c>
+      <c r="Q8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -935,15 +1050,27 @@
       <c r="M9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <v>30</v>
+      </c>
+      <c r="Q9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D10" t="s">
@@ -965,15 +1092,27 @@
         <v>40</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -985,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1136,7 @@
     <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1017,28 +1156,40 @@
         <v>63</v>
       </c>
       <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
         <v>69</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1078,8 +1229,20 @@
       <c r="M2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1119,8 +1282,20 @@
       <c r="M3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1160,8 +1335,20 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1201,8 +1388,20 @@
       <c r="M5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1242,8 +1441,20 @@
       <c r="M6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1283,8 +1494,20 @@
       <c r="M7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1324,8 +1547,20 @@
       <c r="M8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1365,8 +1600,20 @@
       <c r="M9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1406,8 +1653,20 @@
       <c r="M10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1447,8 +1706,20 @@
       <c r="M11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1488,8 +1759,20 @@
       <c r="M12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1502,17 +1785,17 @@
       <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13" t="s">
         <v>27</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1525,17 +1808,17 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H14" t="s">
         <v>27</v>
       </c>
       <c r="L14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1545,14 +1828,14 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1562,14 +1845,14 @@
       <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1579,14 +1862,14 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1599,17 +1882,17 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="G18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="H18" t="s">
         <v>27</v>
       </c>
       <c r="L18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1622,17 +1905,17 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="H19" t="s">
         <v>27</v>
       </c>
       <c r="L19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1645,17 +1928,17 @@
       <c r="D20" t="s">
         <v>27</v>
       </c>
-      <c r="G20" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="H20" t="s">
         <v>27</v>
       </c>
       <c r="L20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1668,17 +1951,17 @@
       <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="G21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="H21" t="s">
         <v>27</v>
       </c>
       <c r="L21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1691,17 +1974,29 @@
       <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="H22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
         <v>27</v>
       </c>
       <c r="M22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>27</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1714,17 +2009,29 @@
       <c r="E23" t="s">
         <v>27</v>
       </c>
-      <c r="H23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="F23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" t="s">
         <v>27</v>
       </c>
       <c r="M23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>27</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1737,17 +2044,29 @@
       <c r="E24" t="s">
         <v>27</v>
       </c>
-      <c r="H24" t="s">
-        <v>27</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
         <v>27</v>
       </c>
       <c r="M24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1760,17 +2079,29 @@
       <c r="E25" t="s">
         <v>27</v>
       </c>
-      <c r="H25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" t="s">
         <v>27</v>
       </c>
       <c r="M25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>27</v>
+      </c>
+      <c r="P25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1783,17 +2114,29 @@
       <c r="E26" t="s">
         <v>27</v>
       </c>
-      <c r="H26" t="s">
-        <v>27</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
         <v>27</v>
       </c>
       <c r="M26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
+        <v>27</v>
+      </c>
+      <c r="P26" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1806,13 +2149,13 @@
       <c r="E27" t="s">
         <v>27</v>
       </c>
-      <c r="H27" t="s">
-        <v>27</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="I27" t="s">
         <v>27</v>
       </c>
       <c r="M27" t="s">
+        <v>27</v>
+      </c>
+      <c r="P27" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1824,10 +2167,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1836,7 +2179,7 @@
     <col min="2" max="3" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1856,28 +2199,40 @@
         <v>63</v>
       </c>
       <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
         <v>69</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1893,26 +2248,38 @@
       <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
       <c r="H2" t="s">
         <v>27</v>
       </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
       <c r="L2" t="s">
         <v>27</v>
       </c>
       <c r="M2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1952,8 +2319,20 @@
       <c r="M3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1993,8 +2372,20 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -2034,8 +2425,20 @@
       <c r="M5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -2075,8 +2478,20 @@
       <c r="M6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -2116,8 +2531,20 @@
       <c r="M7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2157,8 +2584,20 @@
       <c r="M8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2198,8 +2637,20 @@
       <c r="M9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2237,6 +2688,18 @@
         <v>27</v>
       </c>
       <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2247,20 +2710,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2280,28 +2743,40 @@
         <v>63</v>
       </c>
       <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
         <v>69</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -2341,8 +2816,20 @@
       <c r="M2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -2382,8 +2869,20 @@
       <c r="M3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2423,8 +2922,20 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2464,8 +2975,20 @@
       <c r="M5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2505,8 +3028,20 @@
       <c r="M6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2516,23 +3051,29 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" t="s">
         <v>27</v>
       </c>
       <c r="I7" t="s">
         <v>27</v>
       </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -2542,23 +3083,29 @@
       <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
       <c r="H8" t="s">
         <v>27</v>
       </c>
       <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2598,8 +3145,20 @@
       <c r="M9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -2639,8 +3198,20 @@
       <c r="M10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2680,8 +3251,20 @@
       <c r="M11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2721,8 +3304,20 @@
       <c r="M12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2760,6 +3355,18 @@
         <v>27</v>
       </c>
       <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>